<commit_message>
submission sample code added
</commit_message>
<xml_diff>
--- a/data/IPL2021scores.xlsx
+++ b/data/IPL2021scores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kishan/Desktop/IPL/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBC26D8-421B-C44E-949B-EC9F19A41EC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F800F6-6B3B-6747-B8DA-2065D69E15AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16280" xr2:uid="{E57860DC-D49D-BF47-B86C-83FB12E99AD3}"/>
+    <workbookView xWindow="15120" yWindow="540" windowWidth="14380" windowHeight="16280" xr2:uid="{E57860DC-D49D-BF47-B86C-83FB12E99AD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="19">
   <si>
     <t>Matchid</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>RR</t>
+  </si>
+  <si>
+    <t>Batsman</t>
+  </si>
+  <si>
+    <t>Bowlers</t>
+  </si>
+  <si>
+    <t>Get list of bowlers from script</t>
   </si>
 </sst>
 </file>
@@ -443,15 +452,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E046823-5248-AD4C-B2B6-F98BA318EAA8}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,8 +479,17 @@
       <c r="F1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -491,7 +509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -511,7 +529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -531,7 +549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -551,7 +569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -571,7 +589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -591,7 +609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -611,7 +629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>4</v>
       </c>
@@ -631,7 +649,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>5</v>
       </c>
@@ -651,7 +669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>5</v>
       </c>
@@ -671,7 +689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>6</v>
       </c>
@@ -691,7 +709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>6</v>
       </c>
@@ -711,7 +729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>7</v>
       </c>
@@ -731,7 +749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>7</v>
       </c>
@@ -751,7 +769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
28 apr changed last n
</commit_message>
<xml_diff>
--- a/data/IPL2021scores.xlsx
+++ b/data/IPL2021scores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kishan/Desktop/IPL/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F800F6-6B3B-6747-B8DA-2065D69E15AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D610A380-F3CD-554C-B488-7A9A710931A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15120" yWindow="540" windowWidth="14380" windowHeight="16280" xr2:uid="{E57860DC-D49D-BF47-B86C-83FB12E99AD3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{E57860DC-D49D-BF47-B86C-83FB12E99AD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="16">
   <si>
     <t>Matchid</t>
   </si>
@@ -85,15 +85,6 @@
   </si>
   <si>
     <t>RR</t>
-  </si>
-  <si>
-    <t>Batsman</t>
-  </si>
-  <si>
-    <t>Bowlers</t>
-  </si>
-  <si>
-    <t>Get list of bowlers from script</t>
   </si>
 </sst>
 </file>
@@ -452,15 +443,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E046823-5248-AD4C-B2B6-F98BA318EAA8}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,17 +470,8 @@
       <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -509,7 +491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -529,7 +511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -549,7 +531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -569,7 +551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -589,7 +571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -609,7 +591,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -629,7 +611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>4</v>
       </c>
@@ -649,7 +631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>5</v>
       </c>
@@ -669,7 +651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>5</v>
       </c>
@@ -689,7 +671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>6</v>
       </c>
@@ -709,7 +691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>6</v>
       </c>
@@ -729,7 +711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>7</v>
       </c>
@@ -749,7 +731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>7</v>
       </c>
@@ -769,7 +751,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>8</v>
       </c>

</xml_diff>